<commit_message>
Started fixing failed tests
</commit_message>
<xml_diff>
--- a/data/opdracht_template.xlsx
+++ b/data/opdracht_template.xlsx
@@ -16,90 +16,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="189">
   <si>
     <t>naam</t>
   </si>
   <si>
-    <t>opdrachtgever-choice_1-naam</t>
+    <t>opdrachtgever-naam</t>
+  </si>
+  <si>
+    <t>opdrachtgever</t>
+  </si>
+  <si>
+    <t>opdrachtnemer-naam</t>
+  </si>
+  <si>
+    <t>opdrachtnemer</t>
+  </si>
+  <si>
+    <t>dataleverancier-naam</t>
+  </si>
+  <si>
+    <t>dataleverancier</t>
+  </si>
+  <si>
+    <t>kwaliteit-aard</t>
+  </si>
+  <si>
+    <t>aard</t>
+  </si>
+  <si>
+    <t>kwaliteit-origine</t>
+  </si>
+  <si>
+    <t>origine</t>
+  </si>
+  <si>
+    <t>kwaliteit</t>
+  </si>
+  <si>
+    <t>startdatum</t>
+  </si>
+  <si>
+    <t>einddatum</t>
+  </si>
+  <si>
+    <t>omschrijving</t>
+  </si>
+  <si>
+    <t>locatie-coordinatenstelsel</t>
+  </si>
+  <si>
+    <t>coordinatenstelsel</t>
+  </si>
+  <si>
+    <t>locatie-wkt</t>
+  </si>
+  <si>
+    <t>wkt</t>
+  </si>
+  <si>
+    <t>locatie</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>bijlage-titel</t>
+  </si>
+  <si>
+    <t>titel</t>
+  </si>
+  <si>
+    <t>bijlage-choice_1-datum</t>
+  </si>
+  <si>
+    <t>datum</t>
+  </si>
+  <si>
+    <t>bijlage-choice_1-jaar</t>
+  </si>
+  <si>
+    <t>jaar</t>
   </si>
   <si>
     <t>choice_1</t>
   </si>
   <si>
-    <t>opdrachtgever</t>
-  </si>
-  <si>
-    <t>opdrachtnemer-choice_1-naam</t>
-  </si>
-  <si>
-    <t>opdrachtnemer</t>
-  </si>
-  <si>
-    <t>dataleverancier-choice_1-naam</t>
-  </si>
-  <si>
-    <t>dataleverancier</t>
-  </si>
-  <si>
-    <t>kwaliteit-aard</t>
-  </si>
-  <si>
-    <t>aard</t>
-  </si>
-  <si>
-    <t>kwaliteit-origine</t>
-  </si>
-  <si>
-    <t>origine</t>
-  </si>
-  <si>
-    <t>kwaliteit</t>
-  </si>
-  <si>
-    <t>startdatum</t>
-  </si>
-  <si>
-    <t>einddatum</t>
-  </si>
-  <si>
-    <t>omschrijving</t>
-  </si>
-  <si>
-    <t>locatie-coordinatenstelsel</t>
-  </si>
-  <si>
-    <t>coordinatenstelsel</t>
-  </si>
-  <si>
-    <t>locatie-wkt</t>
-  </si>
-  <si>
-    <t>wkt</t>
-  </si>
-  <si>
-    <t>locatie</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>bijlage-titel</t>
-  </si>
-  <si>
-    <t>titel</t>
-  </si>
-  <si>
-    <t>bijlage-choice_1-datum</t>
-  </si>
-  <si>
-    <t>datum</t>
-  </si>
-  <si>
-    <t>bijlage-choice_1-jaar</t>
-  </si>
-  <si>
-    <t>jaar</t>
+    <t>bijlage-bijlage_type</t>
+  </si>
+  <si>
+    <t>bijlage_type</t>
   </si>
   <si>
     <t>bijlage-choice_2-bestand</t>
@@ -117,12 +123,6 @@
     <t>choice_2</t>
   </si>
   <si>
-    <t>bijlage-bijlage_type</t>
-  </si>
-  <si>
-    <t>bijlage_type</t>
-  </si>
-  <si>
     <t>bijlage</t>
   </si>
   <si>
@@ -216,6 +216,12 @@
     <t>CTE onderzoek</t>
   </si>
   <si>
+    <t>Grondverzet onderzoek</t>
+  </si>
+  <si>
+    <t>Evaluatie tijdelijk handelingskader PFAS</t>
+  </si>
+  <si>
     <t>Code</t>
   </si>
   <si>
@@ -264,6 +270,9 @@
     <t>andere</t>
   </si>
   <si>
+    <t>VLAREBO</t>
+  </si>
+  <si>
     <t>geometrie coördinatenstelsel</t>
   </si>
   <si>
@@ -294,196 +303,274 @@
     <t>jaar bijlage</t>
   </si>
   <si>
+    <t>type bijlage</t>
+  </si>
+  <si>
+    <t>edov</t>
+  </si>
+  <si>
+    <t>detailplan</t>
+  </si>
+  <si>
+    <t>foto</t>
+  </si>
+  <si>
+    <t>lithoprofiel</t>
+  </si>
+  <si>
+    <t>korrelverdeling</t>
+  </si>
+  <si>
+    <t>geologisch profiel</t>
+  </si>
+  <si>
+    <t>stijghoogtereeks</t>
+  </si>
+  <si>
+    <t>grondwater kwaliteitsanalyse</t>
+  </si>
+  <si>
+    <t>onttrekking-reeks</t>
+  </si>
+  <si>
+    <t>boorgatmeting</t>
+  </si>
+  <si>
+    <t>attest opvulling put</t>
+  </si>
+  <si>
+    <t>IMJV</t>
+  </si>
+  <si>
+    <t>liggingsplan putten</t>
+  </si>
+  <si>
+    <t>boorrapport</t>
+  </si>
+  <si>
+    <t>putschema</t>
+  </si>
+  <si>
+    <t>vergunning</t>
+  </si>
+  <si>
+    <t>UG-Biblio</t>
+  </si>
+  <si>
+    <t>statusmotivatie</t>
+  </si>
+  <si>
+    <t>UG-Lib</t>
+  </si>
+  <si>
+    <t>kwaliteitscontrole XYZ</t>
+  </si>
+  <si>
+    <t>Data aardkundig profiel</t>
+  </si>
+  <si>
+    <t>Andere archeologie</t>
+  </si>
+  <si>
+    <t>foto bodem omgeving</t>
+  </si>
+  <si>
+    <t>foto bodem profiel zonder nummering</t>
+  </si>
+  <si>
+    <t>foto bodem profiel met nummering</t>
+  </si>
+  <si>
+    <t>archeologische prospectie</t>
+  </si>
+  <si>
+    <t>archeologische opgraving</t>
+  </si>
+  <si>
+    <t>bodemprofielbeschrijving</t>
+  </si>
+  <si>
+    <t>bodemobservaties</t>
+  </si>
+  <si>
+    <t>foto bodem overzicht</t>
+  </si>
+  <si>
+    <t>foto bodem detail</t>
+  </si>
+  <si>
+    <t>foto bodem horizontale coupe</t>
+  </si>
+  <si>
+    <t>bodemexcursiegids</t>
+  </si>
+  <si>
+    <t>rapport</t>
+  </si>
+  <si>
+    <t>sondeerrapport</t>
+  </si>
+  <si>
+    <t>CTE-vooronderzoek</t>
+  </si>
+  <si>
+    <t>CTE-probleemanalyse</t>
+  </si>
+  <si>
+    <t>CTE-oppervlaktedetectie</t>
+  </si>
+  <si>
+    <t>CTE-dieptedetectie</t>
+  </si>
+  <si>
+    <t>CTE-opsporen van CTE</t>
+  </si>
+  <si>
+    <t>CTE-toevalsvondsten</t>
+  </si>
+  <si>
+    <t>CTE-pers</t>
+  </si>
+  <si>
+    <t>Bemalingsstudie</t>
+  </si>
+  <si>
+    <t>BGD-scan</t>
+  </si>
+  <si>
+    <t>BGD-txt</t>
+  </si>
+  <si>
+    <t>fiche herstellingen put/filter</t>
+  </si>
+  <si>
+    <t>GEF bestand</t>
+  </si>
+  <si>
+    <t>Grondwater - advies</t>
+  </si>
+  <si>
+    <t>Grondwater onttrekking-reeks</t>
+  </si>
+  <si>
+    <t>Laboverslag</t>
+  </si>
+  <si>
+    <t>Ontginning - adviezen</t>
+  </si>
+  <si>
+    <t>Ontginning - besluiten</t>
+  </si>
+  <si>
+    <t>Ontginning - schouwingsverslagen</t>
+  </si>
+  <si>
+    <t>Ontginning – werkplan</t>
+  </si>
+  <si>
+    <t>toegangsplan</t>
+  </si>
+  <si>
+    <t>vergunningsbesluit</t>
+  </si>
+  <si>
+    <t>Onderkenningsproeven</t>
+  </si>
+  <si>
+    <t>Volumemassa &amp; watergehalte</t>
+  </si>
+  <si>
+    <t>Steenkool</t>
+  </si>
+  <si>
+    <t>Mech. proeven - CRS</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Schuifweerstandskarakteristieken</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Versterkte proctorproef</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Samendrukking</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Schuifweerstand CD</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Schuifweerstand CU</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Schuifweerstand</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Schuifweerstand UC</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Schuifweerstand UU</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Vinproef</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Vrije prismaproef</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Zwelproef</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Doorlatendheid CV</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Doorlatendheidsproef - algemeen</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Doorlatendheid</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Samendrukkingsproef</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Doorlatendheid VVH</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Doorlatendheid VVV</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Doorlatendheid in tx cel</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Meest losse pakking</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Advanced Triaxiaal testing</t>
+  </si>
+  <si>
+    <t>Mech. proeven - Standaard proctorproef</t>
+  </si>
+  <si>
+    <t>Grondverzet - Technisch verslag</t>
+  </si>
+  <si>
     <t>bestand bijlage</t>
   </si>
   <si>
     <t>URL bijlage</t>
   </si>
   <si>
-    <t>type bijlage</t>
-  </si>
-  <si>
-    <t>edov</t>
-  </si>
-  <si>
-    <t>detailplan</t>
-  </si>
-  <si>
-    <t>foto</t>
-  </si>
-  <si>
-    <t>lithoprofiel</t>
-  </si>
-  <si>
-    <t>korrelverdeling</t>
-  </si>
-  <si>
-    <t>geologisch profiel</t>
-  </si>
-  <si>
-    <t>stijghoogtereeks</t>
-  </si>
-  <si>
-    <t>grondwater kwaliteitsanalyse</t>
-  </si>
-  <si>
-    <t>onttrekking-reeks</t>
-  </si>
-  <si>
-    <t>boorgatmeting</t>
-  </si>
-  <si>
-    <t>attest opvulling put</t>
-  </si>
-  <si>
-    <t>IMJV</t>
-  </si>
-  <si>
-    <t>liggingsplan putten</t>
-  </si>
-  <si>
-    <t>boorrapport</t>
-  </si>
-  <si>
-    <t>putschema</t>
-  </si>
-  <si>
-    <t>vergunning</t>
-  </si>
-  <si>
-    <t>UG-Biblio</t>
-  </si>
-  <si>
-    <t>statusmotivatie</t>
-  </si>
-  <si>
-    <t>UG-Lib</t>
-  </si>
-  <si>
-    <t>kwaliteitscontrole XYZ</t>
-  </si>
-  <si>
-    <t>Data aardkundig profiel</t>
-  </si>
-  <si>
-    <t>Andere archeologie</t>
-  </si>
-  <si>
-    <t>foto bodem omgeving</t>
-  </si>
-  <si>
-    <t>foto bodem profiel zonder nummering</t>
-  </si>
-  <si>
-    <t>foto bodem profiel met nummering</t>
-  </si>
-  <si>
-    <t>archeologische prospectie</t>
-  </si>
-  <si>
-    <t>archeologische opgraving</t>
-  </si>
-  <si>
-    <t>bodemprofielbeschrijving</t>
-  </si>
-  <si>
-    <t>bodemobservaties</t>
-  </si>
-  <si>
-    <t>foto bodem overzicht</t>
-  </si>
-  <si>
-    <t>foto bodem detail</t>
-  </si>
-  <si>
-    <t>foto bodem horizontale coupe</t>
-  </si>
-  <si>
-    <t>bodemexcursiegids</t>
-  </si>
-  <si>
-    <t>rapport</t>
-  </si>
-  <si>
-    <t>sondeerrapport</t>
-  </si>
-  <si>
-    <t>CTE-vooronderzoek</t>
-  </si>
-  <si>
-    <t>CTE-probleemanalyse</t>
-  </si>
-  <si>
-    <t>CTE-oppervlaktedetectie</t>
-  </si>
-  <si>
-    <t>CTE-dieptedetectie</t>
-  </si>
-  <si>
-    <t>CTE-opsporen van CTE</t>
-  </si>
-  <si>
-    <t>CTE-toevalsvondsten</t>
-  </si>
-  <si>
-    <t>CTE-pers</t>
-  </si>
-  <si>
-    <t>Bemalingsstudie</t>
-  </si>
-  <si>
-    <t>BGD-scan</t>
-  </si>
-  <si>
-    <t>BGD-txt</t>
-  </si>
-  <si>
-    <t>fiche herstellingen put/filter</t>
-  </si>
-  <si>
-    <t>GEF bestand</t>
-  </si>
-  <si>
-    <t>Grondwater - advies</t>
-  </si>
-  <si>
-    <t>Grondwater onttrekking-reeks</t>
-  </si>
-  <si>
-    <t>Laboverslag</t>
-  </si>
-  <si>
-    <t>Ontginning - adviezen</t>
-  </si>
-  <si>
-    <t>Ontginning - besluiten</t>
-  </si>
-  <si>
-    <t>Ontginning - schouwingsverslagen</t>
-  </si>
-  <si>
-    <t>Ontginning – werkplan</t>
-  </si>
-  <si>
-    <t>toegangsplan</t>
-  </si>
-  <si>
-    <t>vergunningsbesluit</t>
-  </si>
-  <si>
     <t>opdracht</t>
   </si>
   <si>
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-11-07 19:29:09.409547</t>
+    <t>2024-11-08 01:22:19.717549</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.0.2</t>
+    <t>2.0.3</t>
   </si>
   <si>
     <t>mode</t>
@@ -594,7 +681,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B27" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:B29" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -604,7 +691,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C3:D17" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C3:D18" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -624,7 +711,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="G3:H60" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="G3:H86" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -918,7 +1005,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -929,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -941,46 +1028,46 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -991,19 +1078,19 @@
         <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F4" t="s">
         <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -1017,19 +1104,19 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
         <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -1043,19 +1130,19 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -1069,19 +1156,19 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F7" t="s">
         <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -1095,19 +1182,19 @@
         <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F8" t="s">
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -1121,13 +1208,13 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -1141,13 +1228,13 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
         <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -1161,13 +1248,13 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -1181,13 +1268,13 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -1201,13 +1288,13 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -1221,13 +1308,13 @@
         <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
         <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -1241,13 +1328,13 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
         <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -1261,13 +1348,13 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
         <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -1281,13 +1368,13 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
         <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H17" t="s">
         <v>42</v>
@@ -1300,8 +1387,14 @@
       <c r="B18" t="s">
         <v>42</v>
       </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
       <c r="G18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H18" t="s">
         <v>42</v>
@@ -1315,7 +1408,7 @@
         <v>42</v>
       </c>
       <c r="G19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H19" t="s">
         <v>42</v>
@@ -1329,7 +1422,7 @@
         <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H20" t="s">
         <v>42</v>
@@ -1343,7 +1436,7 @@
         <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H21" t="s">
         <v>42</v>
@@ -1357,7 +1450,7 @@
         <v>42</v>
       </c>
       <c r="G22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H22" t="s">
         <v>42</v>
@@ -1371,7 +1464,7 @@
         <v>42</v>
       </c>
       <c r="G23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H23" t="s">
         <v>42</v>
@@ -1385,7 +1478,7 @@
         <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H24" t="s">
         <v>42</v>
@@ -1399,7 +1492,7 @@
         <v>42</v>
       </c>
       <c r="G25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H25" t="s">
         <v>42</v>
@@ -1413,7 +1506,7 @@
         <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H26" t="s">
         <v>42</v>
@@ -1427,23 +1520,35 @@
         <v>42</v>
       </c>
       <c r="G27" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H27" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
       <c r="G28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H28" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
       <c r="G29" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H29" t="s">
         <v>42</v>
@@ -1451,7 +1556,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="G30" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H30" t="s">
         <v>42</v>
@@ -1459,7 +1564,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="G31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H31" t="s">
         <v>42</v>
@@ -1467,7 +1572,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="G32" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H32" t="s">
         <v>42</v>
@@ -1475,7 +1580,7 @@
     </row>
     <row r="33" spans="7:8">
       <c r="G33" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H33" t="s">
         <v>42</v>
@@ -1483,7 +1588,7 @@
     </row>
     <row r="34" spans="7:8">
       <c r="G34" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H34" t="s">
         <v>42</v>
@@ -1491,7 +1596,7 @@
     </row>
     <row r="35" spans="7:8">
       <c r="G35" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H35" t="s">
         <v>42</v>
@@ -1499,7 +1604,7 @@
     </row>
     <row r="36" spans="7:8">
       <c r="G36" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H36" t="s">
         <v>42</v>
@@ -1507,7 +1612,7 @@
     </row>
     <row r="37" spans="7:8">
       <c r="G37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H37" t="s">
         <v>42</v>
@@ -1515,7 +1620,7 @@
     </row>
     <row r="38" spans="7:8">
       <c r="G38" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H38" t="s">
         <v>42</v>
@@ -1523,7 +1628,7 @@
     </row>
     <row r="39" spans="7:8">
       <c r="G39" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H39" t="s">
         <v>42</v>
@@ -1531,7 +1636,7 @@
     </row>
     <row r="40" spans="7:8">
       <c r="G40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H40" t="s">
         <v>42</v>
@@ -1539,7 +1644,7 @@
     </row>
     <row r="41" spans="7:8">
       <c r="G41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H41" t="s">
         <v>42</v>
@@ -1547,7 +1652,7 @@
     </row>
     <row r="42" spans="7:8">
       <c r="G42" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H42" t="s">
         <v>42</v>
@@ -1555,7 +1660,7 @@
     </row>
     <row r="43" spans="7:8">
       <c r="G43" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H43" t="s">
         <v>42</v>
@@ -1563,7 +1668,7 @@
     </row>
     <row r="44" spans="7:8">
       <c r="G44" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H44" t="s">
         <v>42</v>
@@ -1571,7 +1676,7 @@
     </row>
     <row r="45" spans="7:8">
       <c r="G45" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H45" t="s">
         <v>42</v>
@@ -1579,7 +1684,7 @@
     </row>
     <row r="46" spans="7:8">
       <c r="G46" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H46" t="s">
         <v>42</v>
@@ -1587,7 +1692,7 @@
     </row>
     <row r="47" spans="7:8">
       <c r="G47" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H47" t="s">
         <v>42</v>
@@ -1595,7 +1700,7 @@
     </row>
     <row r="48" spans="7:8">
       <c r="G48" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H48" t="s">
         <v>42</v>
@@ -1603,7 +1708,7 @@
     </row>
     <row r="49" spans="7:8">
       <c r="G49" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H49" t="s">
         <v>42</v>
@@ -1611,7 +1716,7 @@
     </row>
     <row r="50" spans="7:8">
       <c r="G50" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H50" t="s">
         <v>42</v>
@@ -1619,7 +1724,7 @@
     </row>
     <row r="51" spans="7:8">
       <c r="G51" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H51" t="s">
         <v>42</v>
@@ -1627,7 +1732,7 @@
     </row>
     <row r="52" spans="7:8">
       <c r="G52" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H52" t="s">
         <v>42</v>
@@ -1635,7 +1740,7 @@
     </row>
     <row r="53" spans="7:8">
       <c r="G53" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H53" t="s">
         <v>42</v>
@@ -1643,7 +1748,7 @@
     </row>
     <row r="54" spans="7:8">
       <c r="G54" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H54" t="s">
         <v>42</v>
@@ -1651,7 +1756,7 @@
     </row>
     <row r="55" spans="7:8">
       <c r="G55" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H55" t="s">
         <v>42</v>
@@ -1659,7 +1764,7 @@
     </row>
     <row r="56" spans="7:8">
       <c r="G56" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H56" t="s">
         <v>42</v>
@@ -1667,7 +1772,7 @@
     </row>
     <row r="57" spans="7:8">
       <c r="G57" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H57" t="s">
         <v>42</v>
@@ -1675,7 +1780,7 @@
     </row>
     <row r="58" spans="7:8">
       <c r="G58" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H58" t="s">
         <v>42</v>
@@ -1683,7 +1788,7 @@
     </row>
     <row r="59" spans="7:8">
       <c r="G59" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H59" t="s">
         <v>42</v>
@@ -1691,9 +1796,217 @@
     </row>
     <row r="60" spans="7:8">
       <c r="G60" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H60" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="7:8">
+      <c r="G61" t="s">
+        <v>152</v>
+      </c>
+      <c r="H61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="7:8">
+      <c r="G62" t="s">
+        <v>153</v>
+      </c>
+      <c r="H62" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="7:8">
+      <c r="G63" t="s">
+        <v>154</v>
+      </c>
+      <c r="H63" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="7:8">
+      <c r="G64" t="s">
+        <v>155</v>
+      </c>
+      <c r="H64" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="65" spans="7:8">
+      <c r="G65" t="s">
+        <v>156</v>
+      </c>
+      <c r="H65" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="7:8">
+      <c r="G66" t="s">
+        <v>157</v>
+      </c>
+      <c r="H66" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="7:8">
+      <c r="G67" t="s">
+        <v>158</v>
+      </c>
+      <c r="H67" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="7:8">
+      <c r="G68" t="s">
+        <v>159</v>
+      </c>
+      <c r="H68" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="7:8">
+      <c r="G69" t="s">
+        <v>160</v>
+      </c>
+      <c r="H69" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="7:8">
+      <c r="G70" t="s">
+        <v>161</v>
+      </c>
+      <c r="H70" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="71" spans="7:8">
+      <c r="G71" t="s">
+        <v>162</v>
+      </c>
+      <c r="H71" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="7:8">
+      <c r="G72" t="s">
+        <v>163</v>
+      </c>
+      <c r="H72" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="7:8">
+      <c r="G73" t="s">
+        <v>164</v>
+      </c>
+      <c r="H73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="7:8">
+      <c r="G74" t="s">
+        <v>165</v>
+      </c>
+      <c r="H74" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="7:8">
+      <c r="G75" t="s">
+        <v>166</v>
+      </c>
+      <c r="H75" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="76" spans="7:8">
+      <c r="G76" t="s">
+        <v>167</v>
+      </c>
+      <c r="H76" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="7:8">
+      <c r="G77" t="s">
+        <v>168</v>
+      </c>
+      <c r="H77" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="78" spans="7:8">
+      <c r="G78" t="s">
+        <v>169</v>
+      </c>
+      <c r="H78" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="7:8">
+      <c r="G79" t="s">
+        <v>170</v>
+      </c>
+      <c r="H79" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="7:8">
+      <c r="G80" t="s">
+        <v>171</v>
+      </c>
+      <c r="H80" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="7:8">
+      <c r="G81" t="s">
+        <v>172</v>
+      </c>
+      <c r="H81" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="82" spans="7:8">
+      <c r="G82" t="s">
+        <v>173</v>
+      </c>
+      <c r="H82" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="83" spans="7:8">
+      <c r="G83" t="s">
+        <v>174</v>
+      </c>
+      <c r="H83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="7:8">
+      <c r="G84" t="s">
+        <v>175</v>
+      </c>
+      <c r="H84" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="85" spans="7:8">
+      <c r="G85" t="s">
+        <v>176</v>
+      </c>
+      <c r="H85" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="7:8">
+      <c r="G86" t="s">
+        <v>177</v>
+      </c>
+      <c r="H86" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1717,15 +2030,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
-    <col min="2" max="3" width="26.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="36.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" style="3" customWidth="1"/>
@@ -1737,9 +2050,9 @@
     <col min="13" max="13" width="26.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="26.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="24.7109375" style="4" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="30.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="22.7109375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="24.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="24.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="30.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="44.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="36.7109375" style="2" hidden="1" customWidth="1"/>
   </cols>
@@ -1752,43 +2065,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>28</v>
@@ -1797,7 +2110,7 @@
         <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>36</v>
@@ -1811,33 +2124,33 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>35</v>
@@ -1854,40 +2167,40 @@
     </row>
     <row r="3" spans="1:20" hidden="1">
       <c r="B3" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="O3" s="6"/>
-      <c r="P3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="1" t="s">
+      <c r="P3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="R3" s="1"/>
       <c r="S3" s="6" t="s">
         <v>37</v>
       </c>
@@ -1896,88 +2209,78 @@
       </c>
     </row>
     <row r="4" spans="1:20" hidden="1">
-      <c r="B4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>0</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" hidden="1"/>
-    <row r="6" spans="1:20">
-      <c r="A6" s="5" t="s">
+      <c r="R4" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="P6" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="P5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1986,38 +2289,38 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="Q3:R3"/>
     <mergeCell ref="M2:R2"/>
     <mergeCell ref="S2:T2"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E1000001">
-      <formula1>'Codelijsten'!$A$4:$A$27</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E1000001">
+      <formula1>'Codelijsten'!$A$4:$A$29</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F1000001">
-      <formula1>'Codelijsten'!$C$4:$C$17</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F1000001">
+      <formula1>'Codelijsten'!$C$4:$C$18</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7:L1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L1000001">
       <formula1>'Codelijsten'!$E$4:$E$8</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6:N1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R7:R1000001">
-      <formula1>'Codelijsten'!$G$4:$G$60</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P1000001">
+      <formula1>'Codelijsten'!$G$4:$G$86</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E6" location="'Codelijsten'!$A$2" display="aard"/>
-    <hyperlink ref="F6" location="'Codelijsten'!$C$2" display="origine"/>
-    <hyperlink ref="L6" location="'Codelijsten'!$E$2" display="status"/>
-    <hyperlink ref="R6" location="'Codelijsten'!$G$2" display="type bijlage"/>
+    <hyperlink ref="E5" location="'Codelijsten'!$A$2" display="aard"/>
+    <hyperlink ref="F5" location="'Codelijsten'!$C$2" display="origine"/>
+    <hyperlink ref="L5" location="'Codelijsten'!$E$2" display="status"/>
+    <hyperlink ref="P5" location="'Codelijsten'!$G$2" display="type bijlage"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2033,34 +2336,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>